<commit_message>
Updated to search by excel sheet data
</commit_message>
<xml_diff>
--- a/test/testdata/TestData.xlsx
+++ b/test/testdata/TestData.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Cars" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,12 +24,6 @@
     <t>Type of Ad</t>
   </si>
   <si>
-    <t>Min price</t>
-  </si>
-  <si>
-    <t>Max price</t>
-  </si>
-  <si>
     <t>Brand</t>
   </si>
   <si>
@@ -95,6 +88,12 @@
   </si>
   <si>
     <t>Saloon</t>
+  </si>
+  <si>
+    <t>min_price</t>
+  </si>
+  <si>
+    <t>max_price</t>
   </si>
 </sst>
 </file>
@@ -415,7 +414,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,57 +426,57 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
       </c>
       <c r="D2">
         <v>500000</v>
@@ -486,7 +485,7 @@
         <v>1000000</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>1980</v>
@@ -495,16 +494,16 @@
         <v>1990</v>
       </c>
       <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>19</v>
-      </c>
-      <c r="K2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L2" t="s">
-        <v>21</v>
       </c>
       <c r="M2">
         <v>1000</v>
@@ -515,13 +514,13 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
       </c>
       <c r="D3">
         <v>500000</v>
@@ -530,7 +529,7 @@
         <v>1000000</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3">
         <v>1980</v>
@@ -539,16 +538,16 @@
         <v>1990</v>
       </c>
       <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
       <c r="L3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M3">
         <v>1000</v>
@@ -559,13 +558,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
       </c>
       <c r="D4">
         <v>500000</v>
@@ -574,7 +573,7 @@
         <v>1000000</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="G4">
         <v>1970</v>
@@ -583,16 +582,16 @@
         <v>1990</v>
       </c>
       <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>19</v>
-      </c>
-      <c r="K4" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" t="s">
-        <v>21</v>
       </c>
       <c r="M4">
         <v>1000</v>
@@ -603,13 +602,13 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
       </c>
       <c r="D5">
         <v>500000</v>
@@ -618,7 +617,7 @@
         <v>1000000</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G5">
         <v>1980</v>
@@ -627,16 +626,16 @@
         <v>1990</v>
       </c>
       <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" t="s">
         <v>18</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>19</v>
-      </c>
-      <c r="K5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" t="s">
-        <v>21</v>
       </c>
       <c r="M5">
         <v>1000</v>

</xml_diff>